<commit_message>
ЧМ Pract 3 final fixed
</commit_message>
<xml_diff>
--- a/Course III/ЧМ/Pract 3/ЧМ Практика №3.xlsx
+++ b/Course III/ЧМ/Pract 3/ЧМ Практика №3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgiydemo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Disk II/Projects/KIP/Course III/ЧМ/Pract 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="12220" yWindow="460" windowWidth="16580" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -38,18 +38,6 @@
     <t>0.156875</t>
   </si>
   <si>
-    <t>0.646853</t>
-  </si>
-  <si>
-    <t>0.590977</t>
-  </si>
-  <si>
-    <t>1.60212</t>
-  </si>
-  <si>
-    <t>0.760361</t>
-  </si>
-  <si>
     <t>Обратная матрица:</t>
   </si>
   <si>
@@ -69,16 +57,44 @@
   </si>
   <si>
     <t>Деменчук Георгий 3ПКС-115</t>
+  </si>
+  <si>
+    <t>0.663415</t>
+  </si>
+  <si>
+    <t>0.628239</t>
+  </si>
+  <si>
+    <t>1.65558</t>
+  </si>
+  <si>
+    <t>0.553527</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,8 +177,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -183,8 +207,16 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -461,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,7 +521,7 @@
         <v>2.08</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G1" s="5"/>
     </row>
@@ -546,14 +578,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="F5" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -575,7 +607,7 @@
         <v>0.66343622605303865</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,7 +627,7 @@
         <v>0.62827532495966998</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -615,7 +647,7 @@
         <v>1.6556406611920758</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -635,12 +667,12 @@
         <v>0.55353868777279114</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="7"/>
     </row>
@@ -688,15 +720,15 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B15" s="8"/>
       <c r="D15" s="1"/>
       <c r="F15" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -760,13 +792,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>